<commit_message>
Implement multithreading to handle game processing concurrently and prevent server errors.  Added background processing and improved error handling.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/deac259b-70a6-4651-ba4e-72fe6aba6c2c.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,157 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Limbo</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Martin Stig Andersen, Jeppe Carlsen, Thomas Krog, Mads Wibroe, Arnt Jensen, Dino Christian Patti, Stine Sørensen, Morten Christian Bramsen</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2010-07-21</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Limbo is a critically acclaimed 2D puzzle-platformer developed by Playdead, released on July 21, 2010. The game was conceptualized and directed by Arnt Jensen, with significant contributions from developers such as Martin Stig Andersen and Jeppe Carlsen. It was published by Microsoft Studios, Playdead, and 鱼俞 across multiple platforms, including PC, PlayStation, Xbox, and Nintendo Switch. Limbo is celebrated for its minimalist artistic style, which employs a monochrome color palette to create a haunting atmosphere that emphasizes the isolation of its nameless protagonist.
+The gameplay of Limbo revolves around navigating a series of puzzles and platforming challenges in a hostile environment. The game is notable for its use of one-hit deaths, which are mitigated by a generous checkpoint system that encourages experimentation and learning. The player must guide the protagonist through various treacherous environments, using simple controls to manipulate objects and solve physics-based puzzles. Despite its black-and-white aesthetics, the game intuitively distinguishes interactive elements from those that pose danger, ensuring a seamless gameplay experience.
+Limbo's narrative is sparse and open to interpretation, enhancing its enigmatic charm. The game avoids explicit storytelling, instead using its atmospheric design and sound to evoke emotion and tension without relying on traditional horror tropes. This approach, combined with its abrupt ending, has sparked discussions and analysis, contributing to its status as a significant work in the indie gaming scene. The game's sound design, crafted by Andersen, further immerses players in its eerie world, using ambient sounds to heighten suspense and engagement.
+Upon release, Limbo received widespread critical acclaim for its artistic design, innovative gameplay, and unique atmosphere. It earned high praise from various gaming outlets and was recognized with numerous awards, solidifying its position as a milestone in the puzzle-platformer genre. The game's impact extends beyond its immediate success, influencing subsequent indie games with its minimalist approach and atmospheric storytelling.
+Limbo's cultural impact is significant, as it demonstrated the potential of indie games to deliver profound and innovative experiences. Its success helped pave the way for other indie developers to explore unconventional narratives and artistic styles, contributing to a broader acceptance of video games as an art form.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['Edge Staff. (2010, July 23). Limbo review. Edge. https://www.edge-online.com/features/limbo-review', "Herold, C. (2010, July 21). 'Limbo' a haunting, memorable game. The New York Times. https://www.nytimes.com/2010/07/22/arts/video-games/limbo.html", 'Orland, K. (2010, July 20). Review: Limbo. Ars Technica. https://arstechnica.com/gaming/2010/07/review-limbo', 'Parkin, S. (2010, July 19). Limbo review. Eurogamer. https://www.eurogamer.net/articles/2010-07-19-limbo-review', 'Totilo, S. (2010, July 27). The Making of Limbo. Kotaku. https://kotaku.com/the-making-of-limbo-5597437']</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.14
+Average Playtime: 3 hours
+ESRB Rating: Teen
+Metacritic Score: 88
+Platforms: PC, Android, PS Vita, PlayStation 4, PlayStation 3, Xbox 360, Linux, macOS, iOS, Xbox One, Nintendo Switch</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:18:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>422</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Terraria</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Andrew Spinks, Whitney Baird, Victor Moura, Jim Kjexrud, Jamison Hayes, Scott Lloyd Shelly, Chris Bednarz, Yorai Omer</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2011-05-16</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Terraria is a critically acclaimed 2D action-adventure sandbox game initially released on May 16, 2011. Developed by Re-Logic, a company founded by Andrew Spinks, the game combines elements of classic action games with the freedom of sandbox-style creativity. It is available on multiple platforms, including PC, macOS, Linux, and a range of consoles and mobile devices such as Xbox One, PlayStation 4, and Nintendo Switch. The game has been published by several companies over its lifespan, including 505 Games and Spike Chunsoft.
+The gameplay of Terraria revolves around exploration, crafting, building, and combat. Players start by creating a character and entering a randomly generated 2D world filled with diverse biomes, each with unique resources and enemies. The primary goal is to gather materials to craft increasingly powerful weapons and armor, allowing players to tackle more challenging bosses and events. Players can also construct settlements and invite NPCs to inhabit them, which adds depth to the gameplay by providing access to new items and services. The game supports singleplayer and multiplayer modes, with options for cooperative play.
+Terraria's reception has been overwhelmingly positive, praised for its depth, replayability, and the vast array of content available. The pixel-art graphics, combined with a rich soundtrack composed by Scott Lloyd Shelly, contribute to its charming and atmospheric experience. The game's success has led to a thriving modding community, which has further expanded its content and replay value. Terraria has sold millions of copies worldwide, making it one of the best-selling indie games of all time.
+Culturally, Terraria has become a significant part of the indie gaming landscape, often compared to games like Minecraft for its creative freedom and sandbox elements. It has influenced a new generation of sandbox and survival games, encouraging developers to explore similar mechanics and styles. The game's ongoing updates and community support have kept it relevant for over a decade, maintaining a dedicated fanbase and ensuring its place in video game history.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['IGN. (2011). Terraria Review. Retrieved from https://www.ign.com/articles/2011/05/23/terraria-review', 'Metacritic. (n.d.). Terraria for PC Reviews. Retrieved from https://www.metacritic.com/game/pc/terraria', 'PC Gamer. (2011). Terraria Review. Retrieved from https://www.pcgamer.com/terraria-review', 'Polygon. (2020). Terraria: Journey’s End is a perfect goodbye to a decade-old game. Retrieved from https://www.polygon.com/reviews/2020/5/21/21266515/terraria-journeys-end-review-final-update-pc', 'Re-Logic. (n.d.). Official Terraria Website. Retrieved from http://www.terraria.org/']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.06
+Average Playtime: 15 hours
+ESRB Rating: Teen
+Metacritic Score: 81
+Platforms: Xbox 360, Wii U, Nintendo 3DS, Xbox One, PlayStation 4, iOS, PC, macOS, Linux, Nintendo Switch, PlayStation 3, PS Vita, Android</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:19:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3272</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rocket League</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Corey Davis, Thomas Silloway, Bobby McCoin, Sarah Hebbler, Jared Cone</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2015-07-07</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Rocket League is a highly competitive vehicular soccer video game developed and published by Psyonix. Released on July 7, 2015, it is considered a spiritual successor to Psyonix's earlier title, Supersonic Acrobatic Rocket-Powered Battle-Cars. The game quickly gained popularity due to its unique blend of soccer and racing mechanics, offering fast-paced gameplay where players control rocket-powered cars to hit a ball into the opponent's goal. Available on multiple platforms, including Nintendo Switch, Linux, macOS, Xbox One, PC, and PlayStation 4, Rocket League supports various multiplayer modes, including both local and online play, and features cross-platform multiplayer capabilities.
+The game's core mechanics revolve around using rocket-boosted cars to compete in soccer matches. Players can choose from different game modes, ranging from casual matches to competitive ranked play, in team formats such as 1v1, 2v2, and 3v3. The game is renowned for its 'easy to learn, hard to master' mechanics, which are complemented by tight controls, allowing for precise maneuvers and strategic gameplay. Boost pads scattered across the field provide the necessary energy to accelerate or launch cars into the air, enabling advanced aerial techniques. Rocket League also offers extensive customization options, allowing players to personalize their vehicles with various decals, paint jobs, and accessories. Collaborations with popular franchises have introduced iconic vehicles like the Batmobile and the DeLorean from Back to the Future.
+Upon its release, Rocket League received widespread acclaim from critics and players alike, praised for its innovative gameplay, vibrant graphics, and engaging multiplayer experiences. It was lauded for its ability to appeal to both casual players and competitive gamers, leading to a burgeoning esports scene. The game’s soundtrack, featuring a mix of electronic and indie music, also garnered positive feedback for enhancing the gameplay experience. Rocket League's success is reflected in its high player engagement and the passionate community it has cultivated over the years.
+Culturally, Rocket League has had a significant impact on the gaming industry, particularly in the realm of esports. Its inclusion in major esports tournaments and leagues has helped elevate the game's visibility and prestige, solidifying its position as a staple in competitive gaming. The game's cross-platform play feature was a pioneering move that encouraged inclusivity and connectivity among players across different gaming systems. Rocket League's influence extends beyond gaming, as it has become a cultural phenomenon, with its unique concept inspiring a variety of media and merchandise, further embedding it into popular culture.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['IGN Staff. (2015). Rocket League Review. IGN. Retrieved from https://www.ign.com/articles/2015/07/07/rocket-league-review', 'Polygon Staff. (2015). Rocket League is a hit and the new hotness on Twitch. Polygon. Retrieved from https://www.polygon.com/2015/7/10/8929671/rocket-league-sales-twitch-steam', 'GameSpot Staff. (2015). Rocket League Review. GameSpot. Retrieved from https://www.gamespot.com/reviews/rocket-league-review/1900-6416180/', "Tassi, P. (2015). Rocket League's Success Story Is A Tale Of 'Right Place, Right Time'. Forbes. Retrieved from https://www.forbes.com/sites/insertcoin/2015/07/21/rocket-leagues-success-story-is-a-tale-of-right-place-right-time/", 'The Verge Staff. (2016). Rocket League now has more than 19 million players. The Verge. Retrieved from https://www.theverge.com/2016/7/6/12109186/rocket-league-player-count-19-million']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.93
+Average Playtime: 21 hours
+ESRB Rating: Everyone
+Metacritic Score: 86
+Platforms: Nintendo Switch, Linux, macOS, Xbox One, PC, PlayStation 4</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:19:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add game image display to wiki entries and website.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/deac259b-70a6-4651-ba4e-72fe6aba6c2c.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,107 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9767</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hollow Knight</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ari Gibson, David Kazi, Christopher Larkin, William Pellen</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2017-02-23</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Hollow Knight is a critically acclaimed Metroidvania-style action-adventure game developed by the indie studio Team Cherry. Released on February 23, 2017, the game has been lauded for its intricate world design, fluid gameplay mechanics, and atmospheric presentation. Set in the hauntingly beautiful world of Hallownest, players assume the role of the titular Hollow Knight, embarking on a quest to uncover the mysteries of a forgotten kingdom. Team Cherry, consisting of Ari Gibson, David Kazi, Christopher Larkin, and William Pellen, crafted the game with a strong emphasis on exploration, storytelling, and challenging combat.
+The game's narrative unfolds through environmental storytelling, with lore and plot details revealed via in-game items, tablets, and the introspective thoughts of other characters. This indirect storytelling approach encourages players to piece together the history and fate of Hallownest as they traverse its expansive underground world. The journey begins in the town of Dirtmouth, above the ruins of Hallownest, where players descend into the depths to seek answers and confront enigmatic foes. The progression is non-linear, requiring players to backtrack and explore previously inaccessible areas as they acquire new abilities and defeat formidable bosses.
+Hollow Knight's gameplay centers around exploration and combat, with players using a nail as their primary weapon. This nail can be upgraded, allowing for attacks in four directions, and players must hone their platforming skills to navigate the game's interconnected areas. The game's design incorporates classic Metroidvania elements such as hidden secrets, challenging enemies, and dynamic environmental changes that occur as the story progresses. Team Cherry's hand-drawn art style and Christopher Larkin's evocative soundtrack further enhance the game's gothic atmosphere, immersing players in a world that is both 'cute' and foreboding.
+Upon release, Hollow Knight received widespread critical acclaim, praised for its depth, artistic direction, and challenging gameplay. It quickly garnered a dedicated fanbase and became a standout title within the indie gaming landscape. The game's success led to its availability on multiple platforms, including PlayStation 4, Linux, macOS, PC, Nintendo Switch, and Xbox One. With a Metascore of 90 out of 100 and a user rating of 4.41, Hollow Knight has been celebrated as a modern classic in the Metroidvania genre.
+Culturally, Hollow Knight has had a significant impact, inspiring a range of fan art, merchandise, and discussions about its rich lore. It has also paved the way for future indie titles by demonstrating the potential for small studios to create impactful, high-quality games. The game's influence is evident in its continued popularity and the anticipation surrounding its upcoming sequel, Hollow Knight: Silksong.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Metacritic. (n.d.). Hollow Knight. Retrieved from https://www.metacritic.com/game/hollow-knight', 'Smith, G. (2017, March 8). Hollow Knight review: A deep, beautiful, and relentlessly tough Metroidvania. PCWorld. Retrieved from https://www.pcworld.com/article/hollow-knight-review.html', 'Crecente, B. (2017, February 24). Hollow Knight is a beautiful, surprisingly tough Metroidvania. Polygon. Retrieved from https://www.polygon.com/reviews/hollow-knight-review', 'Sinclair, B. (2017, March 11). The making of Hollow Knight. GamesIndustry.biz. Retrieved from https://www.gamesindustry.biz/articles/2017-03-11-the-making-of-hollow-knight', 'Official Hollow Knight Website. (n.d.). Retrieved from http://hollowknight.com']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.41
+Average Playtime: 7 hours
+ESRB Rating: Everyone 10+
+Metacritic Score: 88
+Platforms: PlayStation 4, Linux, macOS, PC, Nintendo Switch, Xbox One</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:21:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>654</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Stardew Valley</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Eric Barone</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2016-02-25</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Stardew Valley is a critically acclaimed indie simulation role-playing game developed by Eric Barone, also known as ConcernedApe, and published by Chucklefish. Released on February 25, 2016, the game is available on a wide array of platforms, including Nintendo Switch, Xbox One, PC, iOS, macOS, Linux, PlayStation 4, PS Vita, and Android. This open-ended game provides players with a sandbox environment where they take on the role of an office worker who inherits an overgrown farm in the small town of Stardew Valley. The game offers a nostalgic nod to classic farming simulators, most notably the Harvest Moon series, while incorporating modern gameplay mechanics.
+The development of Stardew Valley was a remarkable solo endeavor by Eric Barone, who spent over four years designing, programming, and composing the music for the game. Barone's vision was to create a game that not only paid homage to the beloved farming genre but also expanded upon it with a rich set of features. Players can choose the gender, name, and appearance of their character and select a farm layout that best suits their playstyle. The game's mechanics include farming, fishing, mining, crafting, and building relationships with the town's residents. The absence of a primary goal allows players to explore the world at their own pace, engaging in various activities that provide endless gameplay possibilities.
+Stardew Valley was met with widespread critical acclaim upon its release, earning a 4.4 rating and praised for its engaging gameplay, charming pixel art style, and atmospheric soundtrack. The game quickly became a cultural phenomenon within the indie gaming community, noted for its depth and emotional resonance. The inclusion of multiplayer features allowed friends to co-op on farm tasks, adding a social dimension to the experience. Stardew Valley has been credited with revitalizing the farming simulation genre and inspiring numerous indie developers to pursue their projects.
+Culturally, Stardew Valley has had a significant impact, fostering a dedicated fan base and community. It has been highlighted for its inclusive design, allowing players to engage in same-sex relationships and marriages, which has been appreciated for promoting diversity and representation in gaming. The game's success has led to the development of a board game adaptation and ongoing updates, ensuring its continued relevance in the gaming landscape. The official website, stardewvalley.net, serves as a hub for news, updates, and community engagement, reflecting the game's enduring popularity.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['IGN. (2016). Stardew Valley Review. Retrieved from https://www.ign.com/articles/2016/03/07/stardew-valley-review', 'PC Gamer. (2016). Stardew Valley is a farming RPG with a lot more heart than most. Retrieved from https://www.pcgamer.com/stardew-valley-review/', 'Polygon. (2016). Stardew Valley: An interview with its sole creator. Retrieved from https://www.polygon.com/2016/2/29/11133682/stardew-valley-eric-barone-interview', 'The Guardian. (2016). Stardew Valley: the indie farming game that’s taken root in the gaming community. Retrieved from https://www.theguardian.com/technology/2016/mar/09/stardew-valley-indie-farming-game-eric-barone', 'ConcernedApe. (n.d.). Official Stardew Valley Website. Retrieved from http://www.stardewvalley.net']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.4
+Average Playtime: 13 hours
+ESRB Rating: Everyone 10+
+Metacritic Score: 89
+Platforms: Nintendo Switch, Xbox One, PC, iOS, macOS, Linux, PlayStation 4, PS Vita, Android</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:21:38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve game image handling: Handle missing image URLs and display a placeholder icon if an image is not available.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/deac259b-70a6-4651-ba4e-72fe6aba6c2c.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>Date Added</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Image URL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -530,6 +535,7 @@
           <t>2025-03-27 18:18:32</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -580,6 +586,7 @@
           <t>2025-03-27 18:19:04</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -630,6 +637,7 @@
           <t>2025-03-27 18:19:20</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -681,6 +689,7 @@
           <t>2025-03-27 18:21:14</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -731,6 +740,63 @@
           <t>2025-03-27 18:21:38</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3790</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Outlast</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>J. T. Petty, Hugo Dallaire, Samuel Laflamme, David Chateauneuf, Philippe Morin</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2013-09-03</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Outlast, developed by Red Barrels and released on September 3, 2013, is a psychological horror video game that immerses players into a harrowing experience within the confines of the Mount Massive Asylum. The game was developed by a team including J. T. Petty, Hugo Dallaire, Samuel Laflamme, David Chateauneuf, and Philippe Morin, who collectively pushed the boundaries of indie horror gaming. Outlast is available on multiple platforms, including Linux, macOS, Nintendo Switch, PC, Xbox One, and PlayStation 4, making it accessible to a wide audience of horror enthusiasts.
+The narrative of Outlast follows investigative journalist Miles Upshur as he explores a remote psychiatric hospital to uncover the truth behind inhumane experiments conducted on its patients. The game is notable for its first-person perspective, which amplifies the immersive horror experience. Players are equipped with a night vision camera, which serves as their primary tool to navigate the dark and foreboding environments. This camera, however, requires a continuous supply of batteries, adding an additional layer of tension to the gameplay as players must carefully manage resources while avoiding the asylum's hostile inhabitants.
+Unlike traditional survival horror games, Outlast eschews combat mechanics in favor of a focus on stealth and evasion. Players are required to solve puzzles and locate items to progress, all while being relentlessly pursued by the asylum's dangerous and deranged occupants. The realistic movement animations and strategically placed horror sound effects enhance the feeling of vulnerability and suspense, compelling players to empathize with the protagonist's plight.
+Upon release, Outlast received positive reviews for its atmospheric tension, gripping narrative, and innovative use of visual and sound design to create a sense of dread. It earned a rating of 3.74, praised for its ability to evoke terror without the need for direct combat. The game has been credited with revitalizing interest in the survival horror genre, influencing subsequent titles with its emphasis on psychological horror and narrative-driven gameplay.
+Culturally, Outlast has had a significant impact on the horror gaming landscape, inspiring a wave of similar games that prioritize atmosphere and emotional engagement over traditional action elements. The success of Outlast demonstrated the potential for indie developers to create compelling and commercially successful horror experiences, contributing to a broader appreciation for the genre's storytelling capabilities.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['Red Barrels. (2013). Outlast [Video game]. Red Barrels.', 'Smith, A. (2013). Outlast review. IGN. Retrieved from https://www.ign.com/articles/2013/09/03/outlast-review', 'Jones, M. (2013). The horror of Outlast: An interview with Red Barrels. GameSpot. Retrieved from https://www.gamespot.com/articles/the-horror-of-outlast-an-interview-with-red-barrels-6414145/', "Takahashi, D. (2013). Red Barrels' Outlast: How an indie team made a great horror game. VentureBeat. Retrieved from https://venturebeat.com/2013/09/17/red-barrels-outlast-how-an-indie-team-made-a-great-horror-game/", 'Official website of Red Barrels Games. (n.d.). Retrieved from http://redbarrelsgames.com/']</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.74
+Average Playtime: 3 hours
+ESRB Rating: Mature
+Metacritic Score: 80
+Platforms: Linux, macOS, Nintendo Switch, PC, Xbox One, PlayStation 4</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:27:27</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/9dd/9ddabb34840ea9227556670606cf8ea3.jpg</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Increase daily game processing limit to 800 and improve error handling in wiki generation.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/a892a26a-1ef0-4f51-a291-206d31fc07ac.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,6 +798,222 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>9721</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Garry's Mod</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Garry Newman</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2004-12-24</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Garry's Mod, often abbreviated as GMod, is a sandbox game developed by Garry Newman and published by Valve Corporation. Initially released on December 24, 2004, as a mod for Valve's Source engine, it has since evolved into a standalone game available on platforms such as Linux, macOS, and PC. The game is renowned for its open-ended gameplay, allowing players to manipulate objects and experiment with the engine's physics. Unlike traditional video games, Garry's Mod lacks a predefined plot or gameplay objectives, instead offering a flexible environment where users can create and share their own game modes.
+The gameplay mechanics of Garry's Mod revolve around the player's ability to spawn objects, characters, and weapons from the Source engine, and to interact with them in a virtual space. This flexibility has led to the creation of a vast array of user-generated content, ranging from simple amusement to complex game modes such as Trouble in Terrorist Town, Prop Hunt, and various franchise-inspired scenarios like Star Wars and Lord of the Rings. The game supports both single-player and multiplayer modes, with servers categorized by different game modes to ensure players can easily find and join their desired experiences.
+Garry's Mod has received generally positive reviews, with a rating of 3.8. Critics and players alike praise its innovative approach to user-generated content and its role as a creative outlet for gamers. The game's integration with Steam Workshop has facilitated a thriving community where players can share and download mods, further enhancing the game's replayability and depth. The use of Valve's Anti-Cheat system ensures a fair and enjoyable experience for all players.
+The cultural impact of Garry's Mod is significant, as it has inspired a generation of gamers to explore game design and modding. Many players have used it as a stepping stone into the gaming industry, honing skills in animation, modeling, and level design. As a testament to its enduring popularity, Garry's Mod remains a staple in the sandbox genre, celebrated for its humor, creativity, and the freedom it offers players to express themselves through gameplay. The game's visual style, as depicted in its artwork, reflects a blend of realism and whimsical creativity, which has become a hallmark of its enduring appeal.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>["Newman, G. (2004). Garry's Mod. Facepunch Studios.", "Valve Corporation. (n.d.). Garry's Mod [PC, Linux, macOS].", "Smith, A. (2015). The creative impact of Garry's Mod on the gaming industry. PC Gamer.", "Jones, T. (2020). A decade of sandbox innovation: The legacy of Garry's Mod. Game Informer.", "Brown, J. (2022). User-generated content in video games: A study of Garry's Mod. Journal of Game Design and Development."]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.8
+Average Playtime: 14 hours
+ESRB Rating: Rating Pending
+Platforms: Linux, macOS, PC</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:58:55</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/48c/48cb04ca483be865e3a83119c94e6097.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>13668</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Amnesia: The Dark Descent</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mikko Tarmia, Thomas Grip, Jens Nilsson, Mikael Hedberg, Marc Nicander, Marcus Johansson, Luis Rodero Morales</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2010-09-08</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Amnesia: The Dark Descent is a critically acclaimed survival horror video game developed by Frictional Games and released on September 8, 2010. The game is notable for its atmospheric tension and psychological horror elements, setting a new standard in the genre. It was created by a team including Mikko Tarmia, Thomas Grip, Jens Nilsson, Mikael Hedberg, Marc Nicander, Marcus Johansson, and Luis Rodero Morales. Designed for platforms such as Linux, macOS, and PC, Amnesia: The Dark Descent is revered for its immersive storytelling and innovative gameplay mechanics.
+The game places the player in the role of Daniel, a young man who awakens in an eerie, seemingly deserted castle with no memory of his past. The narrative unfolds through environmental cues, notes, audio logs, and visions, inviting players to unravel the castle’s deep-seated secrets. A significant innovation in the game is the Sanity mechanic, which simulates the psychological impact of the environment on Daniel. His mental state can deteriorate from darkness, unsettling visions, and encounters with horrifying creatures, leading to distorted visual and auditory effects that heighten the sense of dread.
+Amnesia: The Dark Descent challenges players through item-based puzzles and interactive environments, requiring resourcefulness and bravery. The game supports modding, allowing user-generated content to flourish and expand the game's universe. It also features a standalone DLC, Justine, which offers a short yet compelling narrative about a female prisoner with multiple possible endings, further enriching the game’s lore.
+Upon release, Amnesia: The Dark Descent received widespread acclaim for its sound design, story richness, and ability to evoke fear without relying on combat mechanics. It garnered a rating of 3.64 and became a landmark title in the survival horror genre. The game's influence is evident in subsequent indie horror titles, which adopted its emphasis on atmosphere and psychological depth. The Lovecraftian themes and the gothic setting have been praised for their authenticity and immersive quality, contributing to the game's enduring legacy.
+Amnesia: The Dark Descent has left a significant impact on both players and developers, expanding the boundaries of horror in video games. Its success demonstrated the potential for indie developers to create compelling, atmospheric experiences that rival those of major studios.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['Frictional Games. (2010). Amnesia: The Dark Descent [Video game]. Frictional Games.', 'IGN. (2010). Amnesia: The Dark Descent Review. Retrieved from https://www.ign.com/articles/2010/09/08/amnesia-the-dark-descent-review', 'GameSpot. (2010). Amnesia: The Dark Descent Review. Retrieved from https://www.gamespot.com/reviews/amnesia-the-dark-descent-review/1900-6275413/', 'PC Gamer. (2010). Amnesia: The Dark Descent Review. Retrieved from https://www.pcgamer.com/amnesia-the-dark-descent-review/', 'Rock, Paper, Shotgun. (2010). Wot I Think: Amnesia: The Dark Descent. Retrieved from https://www.rockpapershotgun.com/amnesia-the-dark-descent-review', 'Official Amnesia: The Dark Descent Website. Retrieved from http://www.amnesiagame.com']</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.64
+Average Playtime: 2 hours
+ESRB Rating: Mature
+Metacritic Score: 85
+Platforms: Linux, macOS, PC</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-03-27 18:59:06</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/b54/b54598d1d5cc31899f4f0a7e3122a7b0.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>12536</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hellblade: Senua's Sacrifice</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Tameem Antoniades, Rupert Brooker, Joe Nelson, Melanie Hall, Juan Fernandez, Andy LaPlegua, David García, Gavin Costello, Stefano Prosperi, Loong Wei Ding</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2017-08-07</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Hellblade: Senua's Sacrifice is a dark fantasy action-adventure game developed and published by Ninja Theory, released on August 7, 2017. The game is set in a gritty world inspired by Scandinavian and Celtic folklore, featuring eerie landscapes and masked enemies. Players control Senua, a Pict warrior grappling with psychosis, as she embarks on a harrowing journey to Helheim to retrieve the soul of her deceased lover, Dillion. Her quest is not only a physical battle against enemies but also a symbolic exploration of her mental struggles, with the game blurring lines between reality and delusion.
+The gameplay of Hellblade: Senua's Sacrifice combines combat and puzzle-solving elements. Players engage in third-person melee combat against various foes while navigating the environment to solve puzzles that require Senua to "focus" and perceive hidden aspects of her surroundings. The game's use of binaural audio technology immerses players in Senua's experiences, with meticulously recorded voices that guide, deceive, or warn her. Motion capture technology was employed to render Senua's movements and expressions with an emotional authenticity that enhances the storytelling experience.
+Critically acclaimed for its narrative depth and innovative approach to portraying mental health, Hellblade received praise for its audio design and visual fidelity. It was lauded for its sensitive depiction of psychosis, developed in collaboration with neuroscientists and individuals with lived experiences of mental illness. The game won several awards, including a BAFTA for Artistic Achievement, and it has been noted for its impact in raising awareness and understanding of mental health issues within the gaming community.
+Culturally, Hellblade: Senua's Sacrifice has been influential in shifting perceptions about the potential of video games as a medium for addressing complex and serious topics. It challenged conventional gaming narratives by focusing on a female protagonist experiencing a mental health condition, contributing to broader discussions about representation and diversity in video games. Its success has encouraged other developers to explore similar themes, solidifying its status as a landmark title in the action-adventure genre.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>["Antoniades, T., Brooker, R., Nelson, J., Hall, M., Fernandez, J., LaPlegua, A., García, D., Costello, G., Prosperi, S., &amp; Ding, L. W. (2017). Hellblade: Senua's Sacrifice [Video game]. Ninja Theory.", "IGN. (2017). Hellblade: Senua's Sacrifice Review. IGN. Retrieved from https://www.ign.com/articles/2017/08/07/hellblade-senuas-sacrifice-review", "Polygon. (2017). How Ninja Theory made Hellblade: Senua's Sacrifice. Polygon. Retrieved from https://www.polygon.com/features/2017/8/8/16109796/hellblade-making-of-ninja-theory", "GamesRadar. (2017). Hellblade: Senua's Sacrifice review: 'A masterpiece of haunting visuals and sound.' GamesRadar. Retrieved from https://www.gamesradar.com/hellblade-senuas-sacrifice-review/", "Official website of Hellblade: Senua's Sacrifice. Retrieved from http://www.hellblade.com/"]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.23
+Average Playtime: 6 hours
+ESRB Rating: Mature
+Metacritic Score: 83
+Platforms: Xbox One, Nintendo Switch, PlayStation 4, PC</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:05:37</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/63f/63f0e68688cad279ed38cde931dbfcdb.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11147</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ARK: Survival Of The Fittest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2016-03-15</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ARK: Survival of the Fittest, released on March 15, 2016, is a distinctive entry in the multiplayer gaming landscape, designed by Studio Wildcard, the creators of ARK: Survival Evolved. This game represents the first-ever Multiplayer Online Survival Arena (M.O.S.A.), crafted to cater to the rapidly expanding eSports scene. As a spin-off from the popular open-world game ARK: Survival Evolved, SotF introduces players to a high-stakes environment where up to 72 players engage in an intense survival battle. The game emphasizes strategic gameplay as participants form Tribes of one to six members, competing on both unofficial and ranked servers in scenarios that range from swift 30-minute skirmishes to extended three-hour confrontations.
+The gameplay of ARK: Survival of the Fittest is marked by its dynamic survival mechanics and competitive elements. Players begin in a neutral staging area to plan their strategies before descending onto the ARK, a lush and perilous environment teeming with prehistoric creatures. The game features over 30 creatures available for taming and riding at the onset of Early Access, with plans for more at full launch. Players must navigate various strategies, such as racing to the central cache for weapons and resources, hiding in the dense forest, or building an army of dinosaurs to dominate opponents. A shrinking "ring of death" gradually forces all players into closer proximity, ensuring that the tension and conflict escalate as the match progresses.
+The game is equipped with robust eSports features, including dedicated ranking systems, matchmaking, and tournament functionalities, making it accessible to a wide audience. Players can also earn exclusive cosmetic items that are compatible with ARK: Survival Evolved. The auditory experience is enriched by a custom soundtrack from Gareth Coker, known for his work on Ori and the Blind Forest, adding a cinematic quality to the competitive gameplay.
+Despite its innovative approach and rich features, ARK: Survival of the Fittest received a mixed reception, garnering an average rating of 2.59. It was praised for its originality and the exciting potential it brought to the eSports arena, yet faced criticism for gameplay balance issues and technical challenges typical of Early Access releases. Nonetheless, it has contributed to the cultural landscape by blending survival mechanics with competitive eSports, thus influencing subsequent titles in the genre.
+The game is available on multiple platforms, including Android, Linux, macOS, PC, and iOS, supporting both single-player and multiplayer modes. Its development and release underscore the growing intersection of survival games and competitive multiplayer experiences in the digital gaming domain.</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['Studio Wildcard. (2016). ARK: Survival of the Fittest [Video game]. Studio Wildcard.', 'Coker, G. (Composer). (2016). ARK: Survival of the Fittest Original Soundtrack [Soundtrack].', 'IGN. (2016). ARK: Survival of the Fittest Review. Retrieved from https://www.ign.com/articles/2016/03/15/ark-survival-of-the-fittest-review', 'PC Gamer. (2016). ARK: Survival of the Fittest: A New Twist in Battle Royale. Retrieved from https://www.pcgamer.com/ark-survival-of-the-fittest-impressions', 'Polygon. (2016). ARK: Survival of the Fittest: How it Changed the Survival Genre. Retrieved from https://www.polygon.com/2016/03/15/ark-survival-of-the-fittest']</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Average Rating: 2.59
+Average Playtime: 1 hours
+ESRB Rating: Teen
+Platforms: Android, Linux, macOS, PC, iOS</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:05:59</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/095/0953bf01cd4e4dd204aba85489ac9868.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: Ensure all processed games are displayed in the game library by directly reading the latest data from the Excel file.  Improved UI to show total games, page numbers, and recently added games.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/a892a26a-1ef0-4f51-a291-206d31fc07ac.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1014,6 +1014,169 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>326292</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Fall Guys: Ultimate Knockout</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2020-08-04</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Fall Guys: Ultimate Knockout is a massively multiplayer online game developed by Mediatonic and published by Devolver Digital. Released on August 4, 2020, the game quickly gained popularity for its chaotic and comedic take on the battle royale genre. The game is available on multiple platforms, including Xbox One, PlayStation 4, PC, Nintendo Switch, and Xbox Series S/X, and supports cross-platform multiplayer, allowing players from different systems to compete against each other.
+In Fall Guys: Ultimate Knockout, players are thrown into a series of increasingly challenging obstacle courses alongside up to 100 competitors online. The goal is to survive each round's bizarre and whimsical challenges to ultimately emerge as the last contestant standing. The gameplay is characterized by its comically exaggerated physics, where characters bounce, tumble, and stumble their way through each course, adding a layer of unpredictability and humor to the competition. Players can customize their avatars with an array of quirky outfits, ranging from pineapple costumes to bunny hats, further enhancing the game's lighthearted and playful atmosphere.
+Upon release, Fall Guys was met with generally positive reviews, praised for its innovative approach to multiplayer gaming and its entertaining, family-friendly appeal. Critics highlighted the game's colorful and cartoonish art style, which, as shown in the game's artwork, adds to the overall fun and whimsical nature of the title. The game's popularity was further fueled by its social media presence and streaming on platforms like Twitch, where it became a favorite among content creators and viewers alike. The game's success led to it becoming one of the most downloaded titles on PlayStation Plus in its release month.
+Culturally, Fall Guys: Ultimate Knockout made a significant impact by introducing a more accessible and less violent alternative to the traditional battle royale format. It resonated with a broad audience, including both casual and hardcore gamers, and became a social gaming phenomenon. Its influence extended beyond the gaming community, with various brands and celebrities expressing interest in collaborations and cross-promotions, further cementing its place in contemporary gaming culture.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['IGN. (2020). Fall Guys: Ultimate Knockout Review. Retrieved from https://www.ign.com/articles/fall-guys-ultimate-knockout-review', 'Polygon. (2020). Fall Guys is the perfect game for when real life is too real. Retrieved from https://www.polygon.com/fall-guys-review', 'The Verge. (2020). Fall Guys becomes the most downloaded PS Plus game of all time. Retrieved from https://www.theverge.com/2020/8/10/fall-guys-most-downloaded-ps-plus-game', 'GameSpot. (2020). Fall Guys: Ultimate Knockout Review. Retrieved from https://www.gamespot.com/reviews/fall-guys-ultimate-knockout-review/1900-6417520/', 'Mediatonic. (2020). Fall Guys: Ultimate Knockout Official Website. Retrieved from https://fallguys.com/']</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.74
+Average Playtime: 6 hours
+ESRB Rating: Everyone
+Metacritic Score: 80
+Platforms: Xbox One, PlayStation 4, PC, Nintendo Switch, Xbox Series S/X</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:14:46</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/5eb/5eb49eb2fa0738fdb5bacea557b1bc57.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>274755</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hades</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Greg Kasavin, Amir Rao, Darren Korb, Jen Zee, Gavin Simon</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2020-09-17</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Hades is a rogue-like dungeon crawler developed and published by Supergiant Games, released on September 17, 2020. It is available on multiple platforms including PlayStation 5, Xbox Series S/X, PlayStation 4, Nintendo Switch, PC, and Xbox One. The game is notable for blending fast-paced action with deep storytelling and intricate character development, drawing upon the successful elements of Supergiant's previous titles such as Bastion, Transistor, and Pyre.
+In Hades, players assume the role of Zagreus, the immortal Prince of the Underworld, who is determined to escape the clutches of his father, Hades, the god of the dead. As Zagreus, players wield mythic weapons and receive powerful Boons from Olympian gods like Zeus, Athena, and Poseidon to enhance their abilities. The game is designed for high replayability, with each escape attempt offering a unique experience due to the ever-shifting Underworld and the various character builds players can discover. As shown in the game's artwork, the rich, hand-painted environments and an original score by Darren Korb bring the atmospheric Underworld to life.
+The development of Hades was led by Greg Kasavin, Amir Rao, Darren Korb, Jen Zee, and Gavin Simon. The game first entered early access in December 2018, allowing players to provide feedback that shaped its evolution. This iterative development process contributed significantly to its polished final release. The game features a fully-voiced cast and engaging narrative, with players able to befriend gods, ghosts, and monsters, thereby unlocking hundreds of unique story events.
+Hades received widespread critical acclaim for its engaging gameplay, rich narrative, and audio-visual presentation. Reviews praised its deep replayability, character-driven storytelling, and the seamless integration of gameplay and narrative. It has been recognized with numerous awards, including the BAFTA Games Award for Best Game and Best Game Design in 2021. Its cultural impact is reflected not only in its critical success but also in its popularity among players, who have embraced its rich mythology and character depth.
+The game's success underscores the potential of indie games to deliver innovative and high-quality experiences, demonstrating how a small team can compete with larger studios by focusing on creativity and player engagement.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['IGN. (2020). Hades Review. Retrieved from https://www.ign.com/articles/hades-review', 'Polygon. (2020). Hades is an Instant Classic. Retrieved from https://www.polygon.com/reviews/2020/9/17/hades-review', "Kasavin, G. (2020). Supergiant's Approach to Developing Hades. GDC Conference.", 'GameSpot. (2020). Why Hades is a Must-Play Game. Retrieved from https://www.gamespot.com/articles/why-hades-is-a-must-play-game/1100-6482730/', 'Eurogamer. (2021). Hades Wins Big at the BAFTA Games Awards. Retrieved from https://www.eurogamer.net/hades-wins-big-at-bafta-games-awards']</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.44
+Average Playtime: 10 hours
+ESRB Rating: Teen
+Metacritic Score: 93
+Platforms: PlayStation 5, Xbox Series S/X, PlayStation 4, Nintendo Switch, PC, Xbox One</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:15:02</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/1f4/1f47a270b8f241e4676b14d39ec620f7.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>22509</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Minecraft</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jens Bergensten, Daniel C418 Rosenfeld, Henrik "carnalizer" Pettersson, Markus Persson, Markus "Junkboy" Toivonen, Jon Kågström, Aron Nieminen, Mattis "Bomb Boy" Grahm, Daniel Frisk</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2009-05-10</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Minecraft is an iconic sandbox video game that was initially released on May 10, 2009. Developed by a team that included notable figures such as Markus Persson and Jens Bergensten, and published by Mojang and Microsoft Studios, Minecraft has become one of the most influential and best-selling games of all time. Available on multiple platforms including Android, iOS, PlayStation, Xbox, and PC, the game is renowned for its open-world design and limitless creative potential.
+The core gameplay of Minecraft revolves around mining resources and crafting items to build various structures. The game's world is procedurally generated and composed of 3D cubes representing different materials and terrains, allowing players to interact with and modify their environment extensively. Players can choose from multiple game modes, including Survival, Creative, and Hardcore. Survival mode challenges players to gather resources, hunt for food, and defend against monsters, while Creative mode offers unlimited resources for unfettered construction and exploration. Hardcore mode introduces permanent death, adding a layer of challenge for seasoned players. Additionally, a multiplayer mode facilitates shared experiences and competitive player-versus-player interactions.
+Minecraft is distinguished by its crude, pixelated visual style, reminiscent of Lego blocks, which has become a cultural icon in its own right. The game's aesthetic simplicity belies its complex and engaging gameplay mechanics, which have inspired a wide array of myths and fan fiction, such as the legendary but non-existent character Herobrine.
+The reception of Minecraft has been overwhelmingly positive, with a rating of 4.43. Critics and players alike have praised its innovative approach to gaming, its vast creative possibilities, and its engaging, community-driven multiplayer aspect. The game has also had a significant cultural impact, influencing numerous aspects of popular culture and being integrated into educational settings to teach concepts ranging from mathematics to environmental stewardship.
+As shown in the game's artwork, Minecraft's visual style and gameplay mechanics have made it a staple in the gaming world, fostering a dedicated community of modders and players who continue to expand and shape the game. The official website, classic.minecraft.net, offers an entry point into the expansive world of Minecraft, a game that continues to evolve and captivate new generations of players.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['Persson, M. (2009). *Minecraft*. Mojang.', 'Totilo, S. (2011). *The Minecraft phenomenon*. Kotaku. Retrieved from https://kotaku.com/the-minecraft-phenomenon-5820413', 'IGN Staff. (2011). *Minecraft Review*. IGN. Retrieved from https://www.ign.com/articles/2011/11/24/minecraft-review', 'Schreier, J. (2015). *How Minecraft became the best-selling PC game of all time*. Kotaku. Retrieved from https://kotaku.com/how-minecraft-became-the-best-selling-pc-game-of-all-ti-1696666722', 'GameSpot Staff. (2010). *Minecraft: Game Overview*. GameSpot. Retrieved from https://www.gamespot.com/games/minecraft/']</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.43
+Average Playtime: 26 hours
+ESRB Rating: Everyone 10+
+Metacritic Score: 83
+Platforms: Android, PS Vita, PlayStation 4, PlayStation 3, Xbox 360, Nintendo 3DS, Nintendo Switch, macOS, PC, iOS, Wii U, Xbox One, Linux</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:15:51</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/b4e/b4e4c73d5aa4ec66bbf75375c4847a2b.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve reference formatting and display in game wiki entries.  Added APA style formatting and improved presentation in the UI.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 946b403d-f3de-4c38-805c-c374546d731d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/0608310e-3b1e-4f69-b840-b1e357ce824c/c1a02093-b044-4afd-abf9-547b36b84474.jpg
</commit_message>
<xml_diff>
--- a/data/game_wiki.xlsx
+++ b/data/game_wiki.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1177,6 +1177,225 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>45969</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Warhammer: Vermintide 2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jesper Kyd, Anders De Geer, Robin Hagblom, Matt Ward, Joakim Setterberg, Arvid Nilsson, Erika S. Kling, Robert Bäckström, Peter Nilsson, Joakim Wahlström</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2018-03-08</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Warhammer: Vermintide 2 is a first-person action game developed by Fatshark and released on March 8, 2018. Serving as a sequel to the 2015 title Warhammer: End Times – Vermintide, the game is set in the Warhammer Fantasy universe during the tumultuous period known as The End Times. Players take on the roles of the heroes of Ubersreik, a group of five protagonists who are tasked with combating the malign forces of the Skaven clan Fester and the chaos warband Rotbloods. The game is notable for its emphasis on cooperative multiplayer gameplay, requiring teamwork and strategic coordination among players to succeed.
+The gameplay of Warhammer: Vermintide 2 is structured around 13 missions, divided into three acts. Each mission requires players to select one of the five heroes and proceed from the start to the finish of the level, engaging in combat with large groups of enemies while completing various objectives. Each character in the game has distinct abilities, weapons, and a unique progression system that defines their role within the party. Characters are equipped with a melee weapon, a ranged weapon, an active ability, several passive abilities, and three career paths to choose from. Careers influence the character's stats, available equipment, and abilities. As players progress and complete missions, they earn random pieces of equipment, which improve in quality as the game advances.
+The development of Warhammer: Vermintide 2 involved a team of talented creators, including Jesper Kyd, Anders De Geer, and Robin Hagblom, among others. The game was published by Fatshark and made available on multiple platforms, including Xbox One, PC, and PlayStation 4. Known for its intense and visceral combat, the game integrates elements of action and indie genres, characterized by its cooperative gameplay, violent encounters, and adherence to the Warhammer lore.
+Upon release, Warhammer: Vermintide 2 received generally favorable reviews, with many critics praising its engaging cooperative multiplayer experience and the depth of its combat system. The game was well-received for its atmospheric setting and challenging gameplay, which appealed to both fans of the Warhammer series and newcomers alike. Its cultural impact is evident in its continued popularity within the cooperative gaming community, often highlighted for its immersive and team-oriented gameplay. With a rating of 3.61, the game has maintained a dedicated player base and contributed to the ongoing legacy of the Warhammer franchise.</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['Fatshark. (2018). Warhammer: Vermintide 2 [Video game]. Fatshark.', 'IGN. (2018, March 8). Warhammer: Vermintide 2 review. IGN. Retrieved from https://www.ign.com', 'Polygon. (2018, March 9). Warhammer: Vermintide 2 is a bloody good time. Polygon. Retrieved from https://www.polygon.com', 'GameSpot. (2018, March 8). Warhammer: Vermintide 2 review. GameSpot. Retrieved from https://www.gamespot.com', 'Eurogamer. (2018, March 10). Warhammer: Vermintide 2 review: a grisly, engaging co-op experience. Eurogamer. Retrieved from https://www.eurogamer.net']</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.61
+Average Playtime: 7 hours
+ESRB Rating: Mature
+Metacritic Score: 82
+Platforms: Xbox One, PC, PlayStation 4</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:20:07</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/5be/5bec14622f6faf804a592176577c1347.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>13627</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Undertale</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Toby Fox</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2015-09-14</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Undertale is an independent role-playing game developed by Toby Fox and released on September 14, 2015. The game is available on multiple platforms including Xbox Series S/X, Nintendo Switch, Xbox One, PC, macOS, Linux, PlayStation 4, and PS Vita. It combines traditional RPG mechanics with unique elements such as bullet hell mini-games, creating an innovative gameplay experience that has captivated players worldwide. Undertale's narrative begins with a backstory of two races, humans and monsters, who once coexisted until a war led to the monsters being sealed underground by human mages. The player controls a human child who falls into the monster realm and must navigate their way back to the surface.
+Undertale's gameplay focuses heavily on player choice, with a branching story and multiple endings determined by the player's actions. Players interact with various NPCs and engage in battles that can be approached either peacefully or aggressively. The game features pixelated graphics reminiscent of retro video games, combined with a unique combat system where players can choose to spare or attack their opponents. These choices affect the behavior of monsters and the overall difficulty of encounters, emphasizing the game's theme of morality and consequence.
+The game's reception was overwhelmingly positive, with critics and players alike praising its storytelling, humor, and innovative mechanics. Undertale's soundtrack, also composed by Toby Fox, received particular acclaim for its ability to enhance the emotional depth of the narrative. The game's design and execution have made it a standout title in the indie gaming scene, leading to a strong fanbase and lasting cultural impact.
+Undertale's influence extends beyond the gaming community, with its themes of empathy and choice resonating with a broad audience. The game has inspired a plethora of fan-created content, including art, music, and even memes, further cementing its place in popular culture. As a testament to its enduring appeal, Undertale continues to be referenced in various media and remains a topic of discussion among gaming enthusiasts.
+For more information, visit the official website at [undertale.com](http://undertale.com).</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['Fox, T. (2015). Undertale [Video game]. Toby Fox.', 'PC Gamer. (2015, September 15). Undertale review. Retrieved from https://www.pcgamer.com/undertale-review/', 'IGN. (2015, September 15). Undertale Review. Retrieved from https://www.ign.com/articles/2015/09/15/undertale-review', 'Polygon. (2015, September 21). Undertale is a game where nobody has to get hurt. Retrieved from https://www.polygon.com/2015/9/21/9357025/undertale-review', 'Metacritic. (2015). Undertale Reviews. Retrieved from https://www.metacritic.com/game/pc/undertale']</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.34
+Average Playtime: 5 hours
+ESRB Rating: Everyone 10+
+Metacritic Score: 92
+Platforms: Xbox Series S/X, Nintendo Switch, Xbox One, PC, macOS, Linux, PlayStation 4, PS Vita</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:20:21</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/ffe/ffed87105b14f5beff72ff44a7793fd5.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>18240</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Brothers: A Tale of Two Sons</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Gustaf Grefberg, Josef Fares</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2013-08-07</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Brothers: A Tale of Two Sons is an action-adventure game that blends narrative-driven storytelling with innovative gameplay mechanics, developed by Gustaf Grefberg and Josef Fares. Released on August 7, 2013, and published by 505 Games and Parables Games, this indie title invites players into a fantastical world filled with emotional depth and richly painted environments. Tasked with saving their ailing father, the titular siblings, Naiee and Naia, embark on a quest to retrieve water from the mythical Tree of Life. Their journey traverses a variety of landscapes including villages, mountains, and forests, challenging them with obstacles such as bullies, trolls, and wolves.
+The gameplay of Brothers: A Tale of Two Sons is distinguished by its unique control scheme, requiring players to manipulate both brothers simultaneously using a single controller. This dual-character control system enhances the puzzle-solving elements of the game, encouraging players to coordinate actions between the two characters, such as having one brother distract an enemy while the other sneaks past. The game seamlessly integrates these mechanics into its narrative, offering a fresh and engaging experience that stands out within the adventure genre. The visual style of the game depicts a vivid and atmospheric world that complements its emotional storytelling, supported by a memorable soundtrack that enriches the overall experience.
+Upon release, Brothers: A Tale of Two Sons received critical acclaim for its innovative gameplay, emotional depth, and artistic presentation. It has been praised for its ability to convey a compelling story through gameplay mechanics rather than traditional narrative techniques. The game has won several awards and is often cited as a significant example of how video games can deliver powerful emotional narratives. Its reception among players has been equally positive, with a rating of 4.18 out of 5, and its availability across multiple platforms, including PlayStation 3, Xbox One, iOS, Nintendo Switch, and more, has broadened its reach to a diverse audience.
+Culturally, Brothers: A Tale of Two Sons has contributed to the discourse on the potential of video games as a medium for storytelling. It has been discussed in various academic and industry settings as a case study in narrative design and player engagement. The game's success has also paved the way for its developers to explore new creative projects, solidifying their reputation in the industry. Its impact is reflected in the continued interest and analysis by gaming scholars and enthusiasts alike.
+For more information, the official website can be accessed at [505 Games](https://505games.com/games/brothers/).</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['Fares, J., &amp; Grefberg, G. (2013). Brothers: A Tale of Two Sons [Video game]. 505 Games, Parables Games.', 'Smith, R. (2013). Review: Brothers: A Tale of Two Sons. GameSpot. Retrieved from https://www.gamespot.com/articles/review-brothers-a-tale-of-two-sons/1100-6412817/', 'Johnson, M. (2014). Emotional storytelling in games: An analysis of Brothers: A Tale of Two Sons. Journal of Game Design, 9(3), 45-58.', 'Thompson, C. (2013). How Brothers: A Tale of Two Sons Redefines Co-Op Gameplay. IGN. Retrieved from https://www.ign.com/articles/2013/08/06/how-brothers-a-tale-of-two-sons-redefines-co-op-gameplay', 'Brown, A. (2015). The Artistic Vision of Brothers: A New Take on Narrative and Gameplay. Polygon. Retrieved from https://www.polygon.com/features/2015/8/7/9114917/the-artistic-vision-of-brothers']</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Average Rating: 4.18
+Average Playtime: 3 hours
+ESRB Rating: Teen
+Metacritic Score: 90
+Platforms: PlayStation 3, Xbox One, iOS, Nintendo Switch, Xbox 360, PlayStation 4, Android, PC</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:20:37</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/b6b/b6b20bfc4b34e312dbc8aac53c95a348.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>9830</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Brawlhalla</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2014-04-30</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Brawlhalla is a free-to-play fighting game that incorporates platformer elements, developed by Blue Mammoth Games and published by Ubisoft Entertainment. It was initially released on April 30, 2014, and has since expanded its availability to multiple platforms including Xbox One, Android, iOS, PC, macOS, Nintendo Switch, and PlayStation 4. The game falls under the genres of Action, Casual, Fighting, and Indie, and is known for its accessibility and competitive gameplay.
+The core gameplay of Brawlhalla involves selecting a character from a roster of 39 heroes, a number that continues to grow with regular updates. The objective is to knock opponents off the stage using a combination of simple controls designed to make the game easy to master. Each character is equipped with two weapons and can utilize various boosts that appear on the stage. Characters also possess attributes such as Strength, Dexterity, Defense, and Speed, which define their combat styles and can be slightly customized. The game supports various modes, including online and local multiplayer, cooperative play, and competitive ranked matches, as well as large arena battles featuring multiple opponents.
+Brawlhalla's development began with a focus on creating a highly accessible yet competitive fighting experience. The game supports cross-platform multiplayer, allowing players to compete with others regardless of their gaming system. Its visual style is characterized by vibrant 2D graphics and dynamic stages, some of which feature multiple platforms that change positions during battles. As shown in the game's artwork, Brawlhalla embraces a colorful and cartoonish aesthetic that appeals to a broad audience.
+Reception of Brawlhalla has been generally positive, with players appreciating its free-to-play model and the depth of its combat mechanics. The game has cultivated a dedicated community and has been the subject of numerous competitions and tournaments worldwide, often featuring monetary prizes. With a rating of 3.22, Brawlhalla is recognized for its engaging multiplayer experience and its role in popularizing the platform fighter genre.
+Brawlhalla has made a significant cultural impact by fostering an inclusive and competitive gaming community. The game's emphasis on skill and strategy over complex controls has made it a staple in the esports scene, drawing players from various backgrounds. Official tournaments and community events have further solidified its standing as a prominent title in the fighting game circuit.
+For more information, visit the official website at [Brawlhalla.com](http://www.brawlhalla.com).</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['Blue Mammoth Games. (n.d.). *Brawlhalla*. Retrieved from http://www.brawlhalla.com', 'Ubisoft Entertainment. (2014). *Brawlhalla* [Video game].', 'IGN. (n.d.). *Brawlhalla Review*. Retrieved from https://www.ign.com', 'Metacritic. (n.d.). *Brawlhalla*. Retrieved from https://www.metacritic.com', 'Polygon. (n.d.). *How Brawlhalla became one of the most popular fighting games*. Retrieved from https://www.polygon.com']</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Average Rating: 3.22
+Average Playtime: 2 hours
+ESRB Rating: Everyone 10+
+Platforms: Xbox One, Android, iOS, PC, macOS, Nintendo Switch, PlayStation 4</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2025-03-27 19:20:54</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://media.rawg.io/media/games/35b/35b47c4d85cd6e08f3e2ca43ea5ce7bb.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>